<commit_message>
dnrpa cambios de lectura
</commit_message>
<xml_diff>
--- a/script_DNRPA/files/registroInscripcionAutoNacion.xlsx
+++ b/script_DNRPA/files/registroInscripcionAutoNacion.xlsx
@@ -1093,7 +1093,7 @@
         <v>399</v>
       </c>
       <c r="V8" t="n">
-        <v>3958</v>
+        <v>3959</v>
       </c>
       <c r="W8" t="n">
         <v>465</v>
@@ -1105,7 +1105,7 @@
         <v>459</v>
       </c>
       <c r="Z8" t="n">
-        <v>44324</v>
+        <v>44325</v>
       </c>
     </row>
     <row r="9">

</xml_diff>